<commit_message>
Update Paper & Graph
</commit_message>
<xml_diff>
--- a/Graph.xlsx
+++ b/Graph.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mr Tan\Desktop\for_draft_paper\draft_paper\paper_draft\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Github\paper_draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F663962-7B8D-4F7E-99C1-E80154BC9DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9CD1A9-BA53-4964-8566-921C102C0F93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2625" yWindow="2625" windowWidth="21600" windowHeight="11400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Graph" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="4">
   <si>
     <t>Value 2</t>
   </si>
@@ -991,13 +991,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1072,25 +1072,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,6 +1508,631 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graph!$AG$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>70%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Graph!$AA$2:$AA$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graph!$AG$2:$AG$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B1CD-4595-9BB8-08AAE77FD9E5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graph!$AC$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Graph!$AA$2:$AA$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graph!$AH$2:$AH$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B1CD-4595-9BB8-08AAE77FD9E5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Graph!$AD$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>90%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Graph!$AA$2:$AA$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Graph!$AI$2:$AI$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B1CD-4595-9BB8-08AAE77FD9E5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="381178112"/>
+        <c:axId val="219601552"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="381178112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>NUMBER OF PROBES</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="219601552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="219601552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>BURSTINESS MAX TIME</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> COUNT</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="381178112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.58278040244969376"/>
+          <c:y val="0.88483741615631384"/>
+          <c:w val="0.38834886408683078"/>
+          <c:h val="7.7107565042440582E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1588,6 +2213,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="202">
   <cs:axisTitle>
@@ -2113,6 +2778,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2697,6 +3878,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>711760</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>125605</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>344366</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>120791</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C85C9CF7-5E83-4480-A5F1-F6A48D32EF73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2968,15 +4187,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE128"/>
+  <dimension ref="A1:AR128"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="O4" zoomScale="91" workbookViewId="0">
-      <selection activeCell="Y12" sqref="Y12"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="V13" zoomScale="91" workbookViewId="0">
+      <selection activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:31" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>5000</v>
       </c>
@@ -3028,8 +4247,20 @@
       <c r="AD1" s="3">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG1" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AH1" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AI1" s="3">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3076,14 +4307,26 @@
         <v>4</v>
       </c>
       <c r="AC2" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD2" s="2">
         <v>1</v>
       </c>
       <c r="AE2" s="2"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF2" s="2">
+        <v>100</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3130,14 +4373,33 @@
         <v>4</v>
       </c>
       <c r="AC3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AD3" s="2">
         <v>2</v>
       </c>
       <c r="AE3" s="2"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF3" s="2">
+        <v>250</v>
+      </c>
+      <c r="AG3" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>6</v>
+      </c>
+      <c r="AI3" s="2">
+        <v>2</v>
+      </c>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3184,14 +4446,33 @@
         <v>4</v>
       </c>
       <c r="AC4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AD4" s="2">
         <v>2</v>
       </c>
       <c r="AE4" s="2"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF4" s="2">
+        <v>500</v>
+      </c>
+      <c r="AG4" s="2">
+        <v>4</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="2">
+        <v>6</v>
+      </c>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3244,8 +4525,27 @@
         <v>3</v>
       </c>
       <c r="AE5" s="2"/>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="AG5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3289,17 +4589,29 @@
         <v>5000</v>
       </c>
       <c r="AB6" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AC6" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AD6" s="2">
         <v>3</v>
       </c>
       <c r="AE6" s="2"/>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AG6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>3</v>
+      </c>
+      <c r="AI6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -3346,14 +4658,26 @@
         <v>7</v>
       </c>
       <c r="AC7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AD7" s="2">
         <v>3</v>
       </c>
       <c r="AE7" s="2"/>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF7" s="2">
+        <v>10000</v>
+      </c>
+      <c r="AG7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AH7" s="2">
+        <v>4</v>
+      </c>
+      <c r="AI7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -3397,17 +4721,29 @@
         <v>15000</v>
       </c>
       <c r="AB8" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AC8" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AD8" s="2">
         <v>4</v>
       </c>
       <c r="AE8" s="2"/>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF8" s="2">
+        <v>15000</v>
+      </c>
+      <c r="AG8" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH8" s="2">
+        <v>4</v>
+      </c>
+      <c r="AI8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -3448,7 +4784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -3488,8 +4824,16 @@
       <c r="U10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -3529,8 +4873,16 @@
       <c r="U11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>9</v>
       </c>
@@ -3558,8 +4910,26 @@
       <c r="O12">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10000</v>
       </c>
@@ -3588,7 +4958,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -3617,7 +4987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>0</v>
       </c>
@@ -3646,7 +5016,7 @@
         <v>7992</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1</v>
       </c>
@@ -3675,7 +5045,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3704,7 +5074,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>3</v>
       </c>
@@ -3733,7 +5103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -3762,7 +5132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>5</v>
       </c>
@@ -3791,7 +5161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>6</v>
       </c>
@@ -3820,7 +5190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>7</v>
       </c>
@@ -3849,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>8</v>
       </c>
@@ -3878,7 +5248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>9</v>
       </c>
@@ -3907,7 +5277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1000</v>
       </c>
@@ -3936,7 +5306,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -3965,7 +5335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>0</v>
       </c>
@@ -3994,7 +5364,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>1</v>
       </c>
@@ -4023,7 +5393,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2</v>
       </c>
@@ -4052,7 +5422,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>3</v>
       </c>
@@ -4081,7 +5451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>4</v>
       </c>
@@ -4110,7 +5480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>5</v>
       </c>
@@ -4139,7 +5509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>6</v>
       </c>
@@ -4168,7 +5538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>7</v>
       </c>
@@ -4197,7 +5567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>8</v>
       </c>
@@ -4226,7 +5596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>9</v>
       </c>
@@ -4255,7 +5625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>500</v>
       </c>
@@ -4284,7 +5654,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -4313,7 +5683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>0</v>
       </c>
@@ -4342,7 +5712,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>1</v>
       </c>
@@ -4371,7 +5741,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>2</v>
       </c>
@@ -4400,7 +5770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>3</v>
       </c>
@@ -4429,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>4</v>
       </c>
@@ -4458,7 +5828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>5</v>
       </c>
@@ -4487,7 +5857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>6</v>
       </c>
@@ -4516,7 +5886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>7</v>
       </c>
@@ -4545,7 +5915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>8</v>
       </c>
@@ -4574,7 +5944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>9</v>
       </c>
@@ -4603,7 +5973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>250</v>
       </c>
@@ -4632,7 +6002,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>2</v>
       </c>
@@ -4661,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>0</v>
       </c>
@@ -4690,7 +6060,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>1</v>
       </c>
@@ -4719,7 +6089,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>2</v>
       </c>
@@ -4748,7 +6118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>3</v>
       </c>
@@ -4777,7 +6147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>4</v>
       </c>
@@ -4806,7 +6176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>5</v>
       </c>
@@ -4835,7 +6205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>6</v>
       </c>
@@ -4864,7 +6234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>7</v>
       </c>
@@ -4893,7 +6263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>8</v>
       </c>
@@ -4922,7 +6292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>9</v>
       </c>
@@ -4951,7 +6321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4980,7 +6350,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>2</v>
       </c>
@@ -5009,7 +6379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>0</v>
       </c>
@@ -5038,7 +6408,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>1</v>
       </c>
@@ -5067,7 +6437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>2</v>
       </c>
@@ -5096,7 +6466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>3</v>
       </c>
@@ -5125,7 +6495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>4</v>
       </c>
@@ -5154,7 +6524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>5</v>
       </c>
@@ -5183,7 +6553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>6</v>
       </c>
@@ -5212,7 +6582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>7</v>
       </c>
@@ -5241,7 +6611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>8</v>
       </c>
@@ -5270,7 +6640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>9</v>
       </c>
@@ -5299,7 +6669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>15000</v>
       </c>
@@ -5328,7 +6698,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>2</v>
       </c>
@@ -5357,7 +6727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>0</v>
       </c>
@@ -5386,7 +6756,7 @@
         <v>12035</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>1</v>
       </c>
@@ -5415,7 +6785,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>2</v>
       </c>
@@ -5444,7 +6814,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>3</v>
       </c>
@@ -5473,7 +6843,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>4</v>
       </c>
@@ -5502,7 +6872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>5</v>
       </c>
@@ -5531,7 +6901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>6</v>
       </c>
@@ -5560,7 +6930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>7</v>
       </c>
@@ -5589,7 +6959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>8</v>
       </c>
@@ -5618,7 +6988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>9</v>
       </c>
@@ -5647,7 +7017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>750</v>
       </c>

</xml_diff>